<commit_message>
created a new table summing up atributes.
</commit_message>
<xml_diff>
--- a/Non_financial.xlsx
+++ b/Non_financial.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\Data modeling\Domen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\Sh\demo\demo\demo-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4414FD11-9D74-4F4F-84C5-A25A747A5D6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,10 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1346,7 +1344,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1505,42 +1503,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:AG79" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
-  <autoFilter ref="A1:AG79"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица1" displayName="Таблица1" ref="A1:AG79" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+  <autoFilter ref="A1:AG79" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="33">
-    <tableColumn id="1" name="#" dataDxfId="32"/>
-    <tableColumn id="2" name="OBJECT_ID" dataDxfId="31"/>
-    <tableColumn id="3" name="SYSTEM_ID" dataDxfId="30"/>
-    <tableColumn id="4" name="ACCOUNT_TYPE_ACCOUNT_CLASS" dataDxfId="29"/>
-    <tableColumn id="5" name="ID" dataDxfId="28"/>
-    <tableColumn id="6" name="S_IN" dataDxfId="27"/>
-    <tableColumn id="7" name="S_OUT" dataDxfId="26"/>
-    <tableColumn id="8" name="DT" dataDxfId="25"/>
-    <tableColumn id="9" name="CT" dataDxfId="24"/>
-    <tableColumn id="10" name="BS_IN" dataDxfId="23"/>
-    <tableColumn id="11" name="BS_OUT" dataDxfId="22"/>
-    <tableColumn id="12" name="BDT" dataDxfId="21"/>
-    <tableColumn id="13" name="BCT" dataDxfId="20"/>
-    <tableColumn id="14" name="DEBIT_COUNT" dataDxfId="19"/>
-    <tableColumn id="15" name="CREDIT_COUNT" dataDxfId="18"/>
-    <tableColumn id="16" name="ZERO_1" dataDxfId="17"/>
-    <tableColumn id="17" name="ZERO_2" dataDxfId="16"/>
-    <tableColumn id="18" name="GENERATED_CODE" dataDxfId="15"/>
-    <tableColumn id="19" name="SPECIAL_CODE" dataDxfId="14"/>
-    <tableColumn id="20" name="POST_ADDRESS" dataDxfId="13"/>
-    <tableColumn id="21" name="CONDITIONAL_FIRST_DATE" dataDxfId="12"/>
-    <tableColumn id="22" name="FIRST_DATE" dataDxfId="11"/>
-    <tableColumn id="23" name="QUALITY_CATEGORY" dataDxfId="10"/>
-    <tableColumn id="24" name="CURRENCY" dataDxfId="9"/>
-    <tableColumn id="25" name="REFERENCE_VALUE" dataDxfId="8"/>
-    <tableColumn id="26" name="RISK_GROUP_ACCOUNT_CLASS" dataDxfId="7"/>
-    <tableColumn id="27" name="REG_CHECK" dataDxfId="6"/>
-    <tableColumn id="28" name="NAME" dataDxfId="5"/>
-    <tableColumn id="29" name="FIXED_VALUE" dataDxfId="4"/>
-    <tableColumn id="30" name="MAXSOUT" dataDxfId="3"/>
-    <tableColumn id="31" name="ZERO_3" dataDxfId="2"/>
-    <tableColumn id="32" name="ZERO_4" dataDxfId="1"/>
-    <tableColumn id="33" name="ZERO_5" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="#" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="OBJECT_ID" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="SYSTEM_ID" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="ACCOUNT_TYPE_ACCOUNT_CLASS" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="ID" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="S_IN" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="S_OUT" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="DT" dataDxfId="25"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="CT" dataDxfId="24"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="BS_IN" dataDxfId="23"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="BS_OUT" dataDxfId="22"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="BDT" dataDxfId="21"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="BCT" dataDxfId="20"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="DEBIT_COUNT" dataDxfId="19"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="CREDIT_COUNT" dataDxfId="18"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="ZERO_1" dataDxfId="17"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="ZERO_2" dataDxfId="16"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="GENERATED_CODE" dataDxfId="15"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="SPECIAL_CODE" dataDxfId="14"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="POST_ADDRESS" dataDxfId="13"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="CONDITIONAL_FIRST_DATE" dataDxfId="12"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="FIRST_DATE" dataDxfId="11"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="QUALITY_CATEGORY" dataDxfId="10"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="CURRENCY" dataDxfId="9"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="REFERENCE_VALUE" dataDxfId="8"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="RISK_GROUP_ACCOUNT_CLASS" dataDxfId="7"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="REG_CHECK" dataDxfId="6"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="NAME" dataDxfId="5"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="FIXED_VALUE" dataDxfId="4"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="MAXSOUT" dataDxfId="3"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="ZERO_3" dataDxfId="2"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="ZERO_4" dataDxfId="1"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="ZERO_5" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1842,12 +1840,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>